<commit_message>
Dia 11 de agosto 2021
Me quedo en ese corte haciendo Revision
</commit_message>
<xml_diff>
--- a/Obrador cortes 1.xlsx
+++ b/Obrador cortes 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELJAIDROSO\Documents\GitHub\Cortes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836C3F97-F3C8-4FF3-9D87-F2F45DE86A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885D1A81-6C42-4183-BF22-0E2838D3EA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="264">
   <si>
     <t>OBRADOR ABRIL 201</t>
   </si>
@@ -789,16 +789,34 @@
     <t>B 15922</t>
   </si>
   <si>
-    <t>B 15790</t>
-  </si>
-  <si>
-    <t>B 15791</t>
-  </si>
-  <si>
-    <t>B 15792</t>
-  </si>
-  <si>
-    <t>B 15793</t>
+    <t>B 15923</t>
+  </si>
+  <si>
+    <t>B 16032</t>
+  </si>
+  <si>
+    <t>B 16078</t>
+  </si>
+  <si>
+    <t>B 16190</t>
+  </si>
+  <si>
+    <t>B 16191</t>
+  </si>
+  <si>
+    <t>B 16285</t>
+  </si>
+  <si>
+    <t>B 16033</t>
+  </si>
+  <si>
+    <t>B 16077</t>
+  </si>
+  <si>
+    <t>B 16286</t>
+  </si>
+  <si>
+    <t>B 16384</t>
   </si>
 </sst>
 </file>
@@ -808,7 +826,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -849,13 +867,6 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -956,7 +967,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143:B146"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2656,97 +2667,120 @@
       <c r="B143" s="13" t="s">
         <v>254</v>
       </c>
+      <c r="C143" s="6" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44416</v>
       </c>
-      <c r="B144" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44417</v>
       </c>
       <c r="B145" s="13" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C145" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44418</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44419</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44420</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44421</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44422</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44423</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44424</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44425</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44426</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44427</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44428</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44429</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44430</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44431</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44432</v>
       </c>

</xml_diff>

<commit_message>
17/08/2021 en la noche
</commit_message>
<xml_diff>
--- a/Obrador cortes 1.xlsx
+++ b/Obrador cortes 1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELJAIDROSO\Documents\GitHub\Cortes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HYDRA999\Documents\GitHub\Cortes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885D1A81-6C42-4183-BF22-0E2838D3EA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhXG2pOraH0RXrcmF4jAc68QlsmUA=="/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="272">
   <si>
     <t>OBRADOR ABRIL 201</t>
   </si>
@@ -817,12 +816,36 @@
   </si>
   <si>
     <t>B 16384</t>
+  </si>
+  <si>
+    <t>B 16486</t>
+  </si>
+  <si>
+    <t>B 16609</t>
+  </si>
+  <si>
+    <t>B 16385</t>
+  </si>
+  <si>
+    <t>B 16485</t>
+  </si>
+  <si>
+    <t>B 16731</t>
+  </si>
+  <si>
+    <t>B 16771</t>
+  </si>
+  <si>
+    <t>B 16610</t>
+  </si>
+  <si>
+    <t>B 16730</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -959,6 +982,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -967,7 +991,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1182,11 +1205,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1196,16 +1219,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1534,16 +1557,16 @@
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1892,16 +1915,16 @@
       <c r="C67" s="6"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="10"/>
     </row>
     <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="10"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="13"/>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
@@ -2229,16 +2252,16 @@
     </row>
     <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B101" s="8"/>
-      <c r="C101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
     </row>
     <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="10"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="12"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="12"/>
+      <c r="C102" s="13"/>
     </row>
     <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
@@ -2583,16 +2606,16 @@
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
+      <c r="A135" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B135" s="8"/>
-      <c r="C135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="10"/>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="10"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="12"/>
+      <c r="A136" s="11"/>
+      <c r="B136" s="12"/>
+      <c r="C136" s="13"/>
     </row>
     <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
@@ -2664,7 +2687,7 @@
       <c r="A143" s="1">
         <v>44415</v>
       </c>
-      <c r="B143" s="13" t="s">
+      <c r="B143" s="7" t="s">
         <v>254</v>
       </c>
       <c r="C143" s="6" t="s">
@@ -2686,7 +2709,7 @@
       <c r="A145" s="1">
         <v>44417</v>
       </c>
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="7" t="s">
         <v>256</v>
       </c>
       <c r="C145" s="6" t="s">
@@ -2697,7 +2720,7 @@
       <c r="A146" s="1">
         <v>44418</v>
       </c>
-      <c r="B146" s="13" t="s">
+      <c r="B146" s="7" t="s">
         <v>258</v>
       </c>
       <c r="C146" s="6" t="s">
@@ -2708,7 +2731,7 @@
       <c r="A147" s="1">
         <v>44419</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="7" t="s">
         <v>262</v>
       </c>
       <c r="C147" s="6" t="s">
@@ -2719,132 +2742,183 @@
       <c r="A148" s="1">
         <v>44420</v>
       </c>
-      <c r="B148" s="2"/>
+      <c r="B148" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44421</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B149" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44422</v>
       </c>
-      <c r="B150" s="2"/>
+      <c r="B150" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44423</v>
       </c>
-      <c r="B151" s="2"/>
+      <c r="B151" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44424</v>
       </c>
-      <c r="B152" s="2"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="5"/>
     </row>
     <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44425</v>
       </c>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
     </row>
     <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44426</v>
       </c>
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
     </row>
     <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44427</v>
       </c>
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
     </row>
     <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44428</v>
       </c>
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
     </row>
     <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44429</v>
       </c>
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
     </row>
     <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44430</v>
       </c>
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
     </row>
     <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44431</v>
       </c>
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
     </row>
     <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44432</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44433</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44434</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+    </row>
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44435</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+    </row>
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44436</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+    </row>
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44437</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="5"/>
+      <c r="C165" s="5"/>
+    </row>
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44438</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+    </row>
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44439</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
     </row>
     <row r="177" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>